<commit_message>
SavingSystem_004 (we will hear from it again)
</commit_message>
<xml_diff>
--- a/pythonEngine/Save_001.xlsx
+++ b/pythonEngine/Save_001.xlsx
@@ -1,51 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
-    <sheet name="גיליון2" sheetId="2" r:id="rId2"/>
-    <sheet name="גיליון3" sheetId="3" r:id="rId3"/>
+    <sheet name="גיליון1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="גיליון2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="גיליון3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>#f94886</t>
-  </si>
-  <si>
-    <t>#d9e25f</t>
-  </si>
-  <si>
-    <t>bgColorButtons</t>
-  </si>
-  <si>
-    <t>fgColorButtons</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -64,18 +48,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -365,32 +411,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="30" customWidth="1"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>bgColorButtons</t>
+        </is>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>IzVhN2FlNw==</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>fgColorButtons</t>
+        </is>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>I2I1NzljOA==</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -399,24 +457,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>